<commit_message>
worked a bit on the 'their_price' column in final output
</commit_message>
<xml_diff>
--- a/test_positions_onliner.xlsx
+++ b/test_positions_onliner.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_works\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\parser_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="49">
   <si>
     <t>Швейные машины</t>
   </si>
@@ -493,7 +494,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD10"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2196,4 +2197,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>1007451001</v>
+      </c>
+      <c r="F1">
+        <v>5990</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>36</v>
+      </c>
+      <c r="M1">
+        <v>5</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>5</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>120</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1007457001</v>
+      </c>
+      <c r="F2">
+        <v>7700</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>36</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>120</v>
+      </c>
+      <c r="R2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>